<commit_message>
Admitcard shift extra comma removed
</commit_message>
<xml_diff>
--- a/dataentry/uploaded_excel_files/cgle_2022_tier2.xlsx
+++ b/dataentry/uploaded_excel_files/cgle_2022_tier2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="205">
   <si>
     <t>ac_main_title</t>
   </si>
@@ -641,6 +641,9 @@
   </si>
   <si>
     <t>YES(SSC)</t>
+  </si>
+  <si>
+    <t>10000092508</t>
   </si>
 </sst>
 </file>
@@ -1015,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BT30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1306,8 +1309,8 @@
       <c r="B2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="1">
-        <v>10000092508</v>
+      <c r="C2" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>82</v>
@@ -1364,7 +1367,7 @@
         <v>58</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z2" s="7" t="s">
         <v>191</v>
@@ -1510,7 +1513,7 @@
         <v>58</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z3" s="7" t="s">
         <v>191</v>
@@ -1639,7 +1642,7 @@
         <v>58</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z4" s="7" t="s">
         <v>191</v>
@@ -1749,7 +1752,7 @@
         <v>58</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z5" s="7" t="s">
         <v>191</v>
@@ -1895,7 +1898,7 @@
         <v>58</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z6" s="7" t="s">
         <v>191</v>
@@ -2041,7 +2044,7 @@
         <v>58</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z7" s="7" t="s">
         <v>191</v>
@@ -2170,7 +2173,7 @@
         <v>58</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z8" s="7" t="s">
         <v>191</v>
@@ -2280,7 +2283,7 @@
         <v>58</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z9" s="7" t="s">
         <v>191</v>
@@ -2390,7 +2393,7 @@
         <v>58</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z10" s="7" t="s">
         <v>191</v>
@@ -2500,7 +2503,7 @@
         <v>58</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z11" s="7" t="s">
         <v>191</v>
@@ -2610,7 +2613,7 @@
         <v>58</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z12" s="7" t="s">
         <v>191</v>
@@ -2737,7 +2740,7 @@
         <v>58</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z13" s="7" t="s">
         <v>191</v>
@@ -2864,7 +2867,7 @@
         <v>58</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z14" s="7" t="s">
         <v>191</v>
@@ -2991,7 +2994,7 @@
         <v>58</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z15" s="7" t="s">
         <v>191</v>
@@ -3118,7 +3121,7 @@
         <v>58</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z16" s="7" t="s">
         <v>191</v>
@@ -3245,7 +3248,7 @@
         <v>58</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z17" s="7" t="s">
         <v>191</v>
@@ -3372,7 +3375,7 @@
         <v>58</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z18" s="7" t="s">
         <v>191</v>
@@ -3501,7 +3504,7 @@
         <v>58</v>
       </c>
       <c r="Y19" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z19" s="7" t="s">
         <v>191</v>
@@ -3630,7 +3633,7 @@
         <v>58</v>
       </c>
       <c r="Y20" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z20" s="7" t="s">
         <v>191</v>
@@ -3776,7 +3779,7 @@
         <v>58</v>
       </c>
       <c r="Y21" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z21" s="7" t="s">
         <v>191</v>
@@ -3903,7 +3906,7 @@
         <v>58</v>
       </c>
       <c r="Y22" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z22" s="7" t="s">
         <v>191</v>
@@ -4030,7 +4033,7 @@
         <v>58</v>
       </c>
       <c r="Y23" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z23" s="7" t="s">
         <v>191</v>
@@ -4157,7 +4160,7 @@
         <v>58</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z24" s="7" t="s">
         <v>191</v>
@@ -4284,7 +4287,7 @@
         <v>58</v>
       </c>
       <c r="Y25" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z25" s="7" t="s">
         <v>191</v>
@@ -4411,7 +4414,7 @@
         <v>58</v>
       </c>
       <c r="Y26" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z26" s="7" t="s">
         <v>191</v>
@@ -4521,7 +4524,7 @@
         <v>58</v>
       </c>
       <c r="Y27" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z27" s="7" t="s">
         <v>191</v>
@@ -4631,7 +4634,7 @@
         <v>58</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z28" s="7" t="s">
         <v>191</v>
@@ -4760,7 +4763,7 @@
         <v>58</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z29" s="7" t="s">
         <v>191</v>
@@ -4889,7 +4892,7 @@
         <v>58</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="Z30" s="7" t="s">
         <v>191</v>

</xml_diff>